<commit_message>
Percentile Calculation of MAE
</commit_message>
<xml_diff>
--- a/data_impute_project/data/human.xlsx
+++ b/data_impute_project/data/human.xlsx
@@ -518,10 +518,10 @@
       <c r="D3" t="n">
         <v>-5</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="n">
         <v>11.9</v>
       </c>
-      <c r="F3" t="inlineStr"/>
       <c r="G3" t="n">
         <v>0.71</v>
       </c>
@@ -545,10 +545,10 @@
       <c r="D4" t="n">
         <v>-5.1</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="n">
         <v>11.8</v>
       </c>
-      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
@@ -570,10 +570,10 @@
       <c r="D5" t="n">
         <v>-5.4</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="n">
         <v>12</v>
       </c>
-      <c r="F5" t="inlineStr"/>
       <c r="G5" t="n">
         <v>0.71</v>
       </c>
@@ -620,10 +620,10 @@
       <c r="D7" t="n">
         <v>-4.9</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="n">
         <v>10.1</v>
       </c>
-      <c r="F7" t="inlineStr"/>
       <c r="G7" t="n">
         <v>0.71</v>
       </c>
@@ -674,10 +674,10 @@
       <c r="D9" t="n">
         <v>-7.2</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
         <v>7.5</v>
       </c>
-      <c r="F9" t="inlineStr"/>
       <c r="G9" t="n">
         <v>0.71</v>
       </c>
@@ -701,10 +701,10 @@
       <c r="D10" t="n">
         <v>-7.2</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="n">
         <v>13.3</v>
       </c>
-      <c r="F10" t="inlineStr"/>
       <c r="G10" t="n">
         <v>0.71</v>
       </c>
@@ -728,10 +728,10 @@
       <c r="D11" t="n">
         <v>-8.6</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="n">
         <v>6.1</v>
       </c>
-      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr">
@@ -803,10 +803,10 @@
       <c r="D14" t="n">
         <v>-6.4</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="n">
         <v>10.4</v>
       </c>
-      <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
         <v>0.71</v>
       </c>
@@ -830,10 +830,10 @@
       <c r="D15" t="n">
         <v>-7.7</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="n">
         <v>4.4</v>
       </c>
-      <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
         <v>0.71</v>
       </c>
@@ -857,10 +857,10 @@
       <c r="D16" t="n">
         <v>-4.8</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="n">
         <v>13.7</v>
       </c>
-      <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
         <v>0.71</v>
       </c>
@@ -884,10 +884,10 @@
       <c r="D17" t="n">
         <v>-5.9</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="n">
         <v>12.5</v>
       </c>
-      <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
         <v>0.71</v>
       </c>
@@ -982,10 +982,10 @@
       <c r="D21" t="n">
         <v>-7</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="n">
         <v>11.5</v>
       </c>
-      <c r="F21" t="inlineStr"/>
       <c r="G21" t="n">
         <v>0.71</v>
       </c>
@@ -1009,10 +1009,10 @@
       <c r="D22" t="n">
         <v>-6</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="n">
         <v>11.3</v>
       </c>
-      <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
         <v>0.71</v>
       </c>
@@ -1036,10 +1036,10 @@
       <c r="D23" t="n">
         <v>-6.5</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="n">
         <v>10.3</v>
       </c>
-      <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
         <v>0.71</v>
       </c>
@@ -1063,10 +1063,10 @@
       <c r="D24" t="n">
         <v>-6.1</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="n">
         <v>5.1</v>
       </c>
-      <c r="F24" t="inlineStr"/>
       <c r="G24" t="n">
         <v>0.71</v>
       </c>
@@ -1165,10 +1165,10 @@
       <c r="D28" t="n">
         <v>-6</v>
       </c>
-      <c r="E28" t="n">
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="n">
         <v>11.3</v>
       </c>
-      <c r="F28" t="inlineStr"/>
       <c r="G28" t="n">
         <v>0.71</v>
       </c>
@@ -1192,10 +1192,10 @@
       <c r="D29" t="n">
         <v>-5.4</v>
       </c>
-      <c r="E29" t="n">
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="n">
         <v>11.2</v>
       </c>
-      <c r="F29" t="inlineStr"/>
       <c r="G29" t="n">
         <v>0.71</v>
       </c>
@@ -1315,10 +1315,10 @@
       <c r="D34" t="n">
         <v>-7.2</v>
       </c>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="n">
+      <c r="E34" t="n">
         <v>18.03</v>
       </c>
+      <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="n">
         <v>0.70909</v>
@@ -1365,10 +1365,10 @@
       <c r="D36" t="n">
         <v>-5.7</v>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="n">
+      <c r="E36" t="n">
         <v>17.64</v>
       </c>
+      <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr"/>
       <c r="H36" t="n">
         <v>0.71055</v>
@@ -1392,10 +1392,10 @@
       <c r="D37" t="n">
         <v>-6.4</v>
       </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="n">
+      <c r="E37" t="n">
         <v>17.97</v>
       </c>
+      <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="n">
         <v>0.71067</v>
@@ -1442,10 +1442,10 @@
       <c r="D39" t="n">
         <v>-8.9</v>
       </c>
-      <c r="E39" t="n">
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="n">
         <v>11.3</v>
       </c>
-      <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr"/>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="inlineStr">
@@ -1467,10 +1467,10 @@
       <c r="D40" t="n">
         <v>-5</v>
       </c>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="n">
+      <c r="E40" t="n">
         <v>17.66</v>
       </c>
+      <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr"/>
       <c r="H40" t="n">
         <v>0.71266</v>
@@ -1517,10 +1517,10 @@
       <c r="D42" t="n">
         <v>-5.7</v>
       </c>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="n">
+      <c r="E42" t="n">
         <v>16.43</v>
       </c>
+      <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="n">
         <v>0.7099299999999999</v>
@@ -1544,10 +1544,10 @@
       <c r="D43" t="n">
         <v>-7.4</v>
       </c>
-      <c r="E43" t="n">
+      <c r="E43" t="inlineStr"/>
+      <c r="F43" t="n">
         <v>13.1</v>
       </c>
-      <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr"/>
       <c r="H43" t="inlineStr"/>
       <c r="I43" t="inlineStr">
@@ -1640,10 +1640,10 @@
       <c r="D47" t="n">
         <v>-7.1</v>
       </c>
-      <c r="E47" t="inlineStr"/>
-      <c r="F47" t="n">
+      <c r="E47" t="n">
         <v>17.24</v>
       </c>
+      <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="n">
         <v>0.7105</v>
@@ -1667,10 +1667,10 @@
       <c r="D48" t="n">
         <v>-6.6</v>
       </c>
-      <c r="E48" t="inlineStr"/>
-      <c r="F48" t="n">
+      <c r="E48" t="n">
         <v>17.05</v>
       </c>
+      <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="n">
         <v>0.71122</v>
@@ -1717,10 +1717,10 @@
       <c r="D50" t="n">
         <v>-6.8</v>
       </c>
-      <c r="E50" t="inlineStr"/>
-      <c r="F50" t="n">
+      <c r="E50" t="n">
         <v>17.26</v>
       </c>
+      <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr"/>
       <c r="H50" t="n">
         <v>0.71118</v>
@@ -1744,10 +1744,10 @@
       <c r="D51" t="n">
         <v>-6.1</v>
       </c>
-      <c r="E51" t="inlineStr"/>
-      <c r="F51" t="n">
+      <c r="E51" t="n">
         <v>16.43</v>
       </c>
+      <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="n">
         <v>0.7110300000000001</v>
@@ -1794,10 +1794,10 @@
       <c r="D53" t="n">
         <v>-6.3</v>
       </c>
-      <c r="E53" t="n">
+      <c r="E53" t="inlineStr"/>
+      <c r="F53" t="n">
         <v>7.1</v>
       </c>
-      <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr"/>
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr">
@@ -1819,10 +1819,10 @@
       <c r="D54" t="n">
         <v>-7.9</v>
       </c>
-      <c r="E54" t="inlineStr"/>
-      <c r="F54" t="n">
+      <c r="E54" t="n">
         <v>17.65</v>
       </c>
+      <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr"/>
       <c r="H54" t="n">
         <v>0.70989</v>
@@ -1846,10 +1846,10 @@
       <c r="D55" t="n">
         <v>-6.6</v>
       </c>
-      <c r="E55" t="n">
+      <c r="E55" t="inlineStr"/>
+      <c r="F55" t="n">
         <v>8.6</v>
       </c>
-      <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr">
@@ -1894,10 +1894,10 @@
       <c r="D57" t="n">
         <v>-7.7</v>
       </c>
-      <c r="E57" t="n">
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="n">
         <v>11.5</v>
       </c>
-      <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr"/>
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr">
@@ -1990,10 +1990,10 @@
       <c r="D61" t="n">
         <v>-5.3</v>
       </c>
-      <c r="E61" t="inlineStr"/>
-      <c r="F61" t="n">
+      <c r="E61" t="n">
         <v>17.45</v>
       </c>
+      <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr"/>
       <c r="H61" t="n">
         <v>0.70956</v>
@@ -2040,10 +2040,10 @@
       <c r="D63" t="n">
         <v>-7.9</v>
       </c>
-      <c r="E63" t="n">
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="n">
         <v>9.800000000000001</v>
       </c>
-      <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr"/>
       <c r="H63" t="inlineStr"/>
       <c r="I63" t="inlineStr">
@@ -2065,10 +2065,10 @@
       <c r="D64" t="n">
         <v>-5.3</v>
       </c>
-      <c r="E64" t="inlineStr"/>
-      <c r="F64" t="n">
+      <c r="E64" t="n">
         <v>17.1</v>
       </c>
+      <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="n">
         <v>0.71011</v>
@@ -2092,10 +2092,10 @@
       <c r="D65" t="n">
         <v>-5.4</v>
       </c>
-      <c r="E65" t="inlineStr"/>
-      <c r="F65" t="n">
+      <c r="E65" t="n">
         <v>17.76</v>
       </c>
+      <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr"/>
       <c r="H65" t="n">
         <v>0.71073</v>
@@ -2165,10 +2165,10 @@
       <c r="D68" t="n">
         <v>-8.300000000000001</v>
       </c>
-      <c r="E68" t="n">
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="n">
         <v>11.6</v>
       </c>
-      <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr"/>
       <c r="H68" t="inlineStr"/>
       <c r="I68" t="inlineStr">
@@ -2190,10 +2190,10 @@
       <c r="D69" t="n">
         <v>-8.6</v>
       </c>
-      <c r="E69" t="n">
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="n">
         <v>7.9</v>
       </c>
-      <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr"/>
       <c r="H69" t="inlineStr"/>
       <c r="I69" t="inlineStr">
@@ -2215,10 +2215,10 @@
       <c r="D70" t="n">
         <v>-8.4</v>
       </c>
-      <c r="E70" t="inlineStr"/>
-      <c r="F70" t="n">
+      <c r="E70" t="n">
         <v>16.2</v>
       </c>
+      <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="n">
         <v>0.7107599999999999</v>
@@ -2335,10 +2335,10 @@
         <v>-6.9</v>
       </c>
       <c r="E75" t="n">
+        <v>17.34</v>
+      </c>
+      <c r="F75" t="n">
         <v>6.8</v>
-      </c>
-      <c r="F75" t="n">
-        <v>17.34</v>
       </c>
       <c r="G75" t="inlineStr"/>
       <c r="H75" t="n">
@@ -2386,10 +2386,10 @@
       <c r="D77" t="n">
         <v>-7.5</v>
       </c>
-      <c r="E77" t="n">
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="n">
         <v>11.3</v>
       </c>
-      <c r="F77" t="inlineStr"/>
       <c r="G77" t="inlineStr"/>
       <c r="H77" t="inlineStr"/>
       <c r="I77" t="inlineStr">
@@ -2411,10 +2411,10 @@
       <c r="D78" t="n">
         <v>-8.199999999999999</v>
       </c>
-      <c r="E78" t="n">
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="n">
         <v>9.300000000000001</v>
       </c>
-      <c r="F78" t="inlineStr"/>
       <c r="G78" t="inlineStr"/>
       <c r="H78" t="inlineStr"/>
       <c r="I78" t="inlineStr">
@@ -2459,10 +2459,10 @@
       <c r="D80" t="n">
         <v>-7.7</v>
       </c>
-      <c r="E80" t="n">
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" t="n">
         <v>12.7</v>
       </c>
-      <c r="F80" t="inlineStr"/>
       <c r="G80" t="inlineStr"/>
       <c r="H80" t="inlineStr"/>
       <c r="I80" t="inlineStr">
@@ -2484,10 +2484,10 @@
       <c r="D81" t="n">
         <v>-7.9</v>
       </c>
-      <c r="E81" t="n">
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="n">
         <v>12.7</v>
       </c>
-      <c r="F81" t="inlineStr"/>
       <c r="G81" t="inlineStr"/>
       <c r="H81" t="inlineStr"/>
       <c r="I81" t="inlineStr">
@@ -2555,10 +2555,10 @@
       <c r="D84" t="n">
         <v>-8.5</v>
       </c>
-      <c r="E84" t="n">
+      <c r="E84" t="inlineStr"/>
+      <c r="F84" t="n">
         <v>11.3</v>
       </c>
-      <c r="F84" t="inlineStr"/>
       <c r="G84" t="inlineStr"/>
       <c r="H84" t="inlineStr"/>
       <c r="I84" t="inlineStr">
@@ -2581,10 +2581,10 @@
         <v>-7.3</v>
       </c>
       <c r="E85" t="n">
+        <v>17.78</v>
+      </c>
+      <c r="F85" t="n">
         <v>2.1</v>
-      </c>
-      <c r="F85" t="n">
-        <v>17.78</v>
       </c>
       <c r="G85" t="inlineStr"/>
       <c r="H85" t="n">
@@ -2655,10 +2655,10 @@
       <c r="D88" t="n">
         <v>-8.5</v>
       </c>
-      <c r="E88" t="inlineStr"/>
-      <c r="F88" t="n">
+      <c r="E88" t="n">
         <v>18.35</v>
       </c>
+      <c r="F88" t="inlineStr"/>
       <c r="G88" t="inlineStr"/>
       <c r="H88" t="n">
         <v>0.70941</v>
@@ -2682,10 +2682,10 @@
       <c r="D89" t="n">
         <v>-6.5</v>
       </c>
-      <c r="E89" t="inlineStr"/>
-      <c r="F89" t="n">
+      <c r="E89" t="n">
         <v>17.81</v>
       </c>
+      <c r="F89" t="inlineStr"/>
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="n">
         <v>0.70931</v>
@@ -2732,10 +2732,10 @@
       <c r="D91" t="n">
         <v>-7.2</v>
       </c>
-      <c r="E91" t="inlineStr"/>
-      <c r="F91" t="n">
+      <c r="E91" t="n">
         <v>17.73</v>
       </c>
+      <c r="F91" t="inlineStr"/>
       <c r="G91" t="inlineStr"/>
       <c r="H91" t="n">
         <v>0.7101499999999999</v>
@@ -2759,10 +2759,10 @@
       <c r="D92" t="n">
         <v>-8.699999999999999</v>
       </c>
-      <c r="E92" t="inlineStr"/>
-      <c r="F92" t="n">
+      <c r="E92" t="n">
         <v>16.58</v>
       </c>
+      <c r="F92" t="inlineStr"/>
       <c r="G92" t="inlineStr"/>
       <c r="H92" t="n">
         <v>0.7108</v>
@@ -2809,10 +2809,10 @@
       <c r="D94" t="n">
         <v>-8.5</v>
       </c>
-      <c r="E94" t="n">
+      <c r="E94" t="inlineStr"/>
+      <c r="F94" t="n">
         <v>11.5</v>
       </c>
-      <c r="F94" t="inlineStr"/>
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="n">
         <v>0.70925</v>
@@ -2836,10 +2836,10 @@
       <c r="D95" t="n">
         <v>-6.1</v>
       </c>
-      <c r="E95" t="inlineStr"/>
-      <c r="F95" t="n">
+      <c r="E95" t="n">
         <v>16.81</v>
       </c>
+      <c r="F95" t="inlineStr"/>
       <c r="G95" t="inlineStr"/>
       <c r="H95" t="n">
         <v>0.7092000000000001</v>
@@ -2863,10 +2863,10 @@
       <c r="D96" t="n">
         <v>-8.5</v>
       </c>
-      <c r="E96" t="n">
+      <c r="E96" t="inlineStr"/>
+      <c r="F96" t="n">
         <v>7.7</v>
       </c>
-      <c r="F96" t="inlineStr"/>
       <c r="G96" t="inlineStr"/>
       <c r="H96" t="inlineStr"/>
       <c r="I96" t="inlineStr">
@@ -2889,10 +2889,10 @@
         <v>-7</v>
       </c>
       <c r="E97" t="n">
+        <v>16.48</v>
+      </c>
+      <c r="F97" t="n">
         <v>9.5</v>
-      </c>
-      <c r="F97" t="n">
-        <v>16.48</v>
       </c>
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="n">
@@ -2917,10 +2917,10 @@
       <c r="D98" t="n">
         <v>-7.3</v>
       </c>
-      <c r="E98" t="n">
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="n">
         <v>3.5</v>
       </c>
-      <c r="F98" t="inlineStr"/>
       <c r="G98" t="inlineStr"/>
       <c r="H98" t="inlineStr"/>
       <c r="I98" t="inlineStr">
@@ -2943,10 +2943,10 @@
         <v>-8.1</v>
       </c>
       <c r="E99" t="n">
+        <v>16.78</v>
+      </c>
+      <c r="F99" t="n">
         <v>9.300000000000001</v>
-      </c>
-      <c r="F99" t="n">
-        <v>16.78</v>
       </c>
       <c r="G99" t="inlineStr"/>
       <c r="H99" t="n">
@@ -3043,10 +3043,10 @@
         <v>-7.1</v>
       </c>
       <c r="E103" t="n">
+        <v>16.6</v>
+      </c>
+      <c r="F103" t="n">
         <v>11.4</v>
-      </c>
-      <c r="F103" t="n">
-        <v>16.6</v>
       </c>
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="n">
@@ -3096,10 +3096,10 @@
       <c r="D105" t="n">
         <v>-8</v>
       </c>
-      <c r="E105" t="n">
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="n">
         <v>11.7</v>
       </c>
-      <c r="F105" t="inlineStr"/>
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr"/>
       <c r="I105" t="inlineStr">
@@ -3144,10 +3144,10 @@
       <c r="D107" t="n">
         <v>-8.6</v>
       </c>
-      <c r="E107" t="n">
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="n">
         <v>11.2</v>
       </c>
-      <c r="F107" t="inlineStr"/>
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="inlineStr"/>
       <c r="I107" t="inlineStr">
@@ -3217,10 +3217,10 @@
       <c r="D110" t="n">
         <v>-7.6</v>
       </c>
-      <c r="E110" t="n">
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="n">
         <v>5.8</v>
       </c>
-      <c r="F110" t="inlineStr"/>
       <c r="G110" t="inlineStr"/>
       <c r="H110" t="n">
         <v>0.70933</v>
@@ -3244,10 +3244,10 @@
       <c r="D111" t="n">
         <v>-7.4</v>
       </c>
-      <c r="E111" t="n">
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="n">
         <v>10.2</v>
       </c>
-      <c r="F111" t="inlineStr"/>
       <c r="G111" t="inlineStr"/>
       <c r="H111" t="n">
         <v>0.70933</v>
@@ -3344,10 +3344,10 @@
       <c r="D115" t="n">
         <v>-6.6</v>
       </c>
-      <c r="E115" t="n">
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="n">
         <v>12.8</v>
       </c>
-      <c r="F115" t="inlineStr"/>
       <c r="G115" t="inlineStr"/>
       <c r="H115" t="inlineStr"/>
       <c r="I115" t="inlineStr">
@@ -3369,10 +3369,10 @@
       <c r="D116" t="n">
         <v>-9.199999999999999</v>
       </c>
-      <c r="E116" t="n">
+      <c r="E116" t="inlineStr"/>
+      <c r="F116" t="n">
         <v>10.3</v>
       </c>
-      <c r="F116" t="inlineStr"/>
       <c r="G116" t="inlineStr"/>
       <c r="H116" t="n">
         <v>0.70956</v>
@@ -3396,10 +3396,10 @@
       <c r="D117" t="n">
         <v>-7.6</v>
       </c>
-      <c r="E117" t="n">
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="n">
         <v>9.6</v>
       </c>
-      <c r="F117" t="inlineStr"/>
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr"/>
       <c r="I117" t="inlineStr">
@@ -3421,10 +3421,10 @@
       <c r="D118" t="n">
         <v>-7.7</v>
       </c>
-      <c r="E118" t="n">
+      <c r="E118" t="inlineStr"/>
+      <c r="F118" t="n">
         <v>11</v>
       </c>
-      <c r="F118" t="inlineStr"/>
       <c r="G118" t="inlineStr"/>
       <c r="H118" t="inlineStr"/>
       <c r="I118" t="inlineStr">
@@ -3519,10 +3519,10 @@
       <c r="D122" t="n">
         <v>-8</v>
       </c>
-      <c r="E122" t="n">
+      <c r="E122" t="inlineStr"/>
+      <c r="F122" t="n">
         <v>11.3</v>
       </c>
-      <c r="F122" t="inlineStr"/>
       <c r="G122" t="inlineStr"/>
       <c r="H122" t="inlineStr"/>
       <c r="I122" t="inlineStr">
@@ -3567,10 +3567,10 @@
       <c r="D124" t="n">
         <v>-7.9</v>
       </c>
-      <c r="E124" t="n">
+      <c r="E124" t="inlineStr"/>
+      <c r="F124" t="n">
         <v>2.6</v>
       </c>
-      <c r="F124" t="inlineStr"/>
       <c r="G124" t="inlineStr"/>
       <c r="H124" t="inlineStr"/>
       <c r="I124" t="inlineStr">
@@ -3592,10 +3592,10 @@
       <c r="D125" t="n">
         <v>-8.6</v>
       </c>
-      <c r="E125" t="n">
+      <c r="E125" t="inlineStr"/>
+      <c r="F125" t="n">
         <v>8.9</v>
       </c>
-      <c r="F125" t="inlineStr"/>
       <c r="G125" t="inlineStr"/>
       <c r="H125" t="inlineStr"/>
       <c r="I125" t="inlineStr">
@@ -3617,10 +3617,10 @@
       <c r="D126" t="n">
         <v>-6.8</v>
       </c>
-      <c r="E126" t="n">
+      <c r="E126" t="inlineStr"/>
+      <c r="F126" t="n">
         <v>7.2</v>
       </c>
-      <c r="F126" t="inlineStr"/>
       <c r="G126" t="inlineStr"/>
       <c r="H126" t="inlineStr"/>
       <c r="I126" t="inlineStr">
@@ -3690,10 +3690,10 @@
       <c r="D129" t="n">
         <v>-7.4</v>
       </c>
-      <c r="E129" t="n">
+      <c r="E129" t="inlineStr"/>
+      <c r="F129" t="n">
         <v>10.3</v>
       </c>
-      <c r="F129" t="inlineStr"/>
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr"/>
       <c r="I129" t="inlineStr">
@@ -3740,10 +3740,10 @@
       <c r="D131" t="n">
         <v>-9.300000000000001</v>
       </c>
-      <c r="E131" t="n">
+      <c r="E131" t="inlineStr"/>
+      <c r="F131" t="n">
         <v>6.6</v>
       </c>
-      <c r="F131" t="inlineStr"/>
       <c r="G131" t="inlineStr"/>
       <c r="H131" t="inlineStr"/>
       <c r="I131" t="inlineStr">
@@ -3765,10 +3765,10 @@
       <c r="D132" t="n">
         <v>-8.800000000000001</v>
       </c>
-      <c r="E132" t="n">
+      <c r="E132" t="inlineStr"/>
+      <c r="F132" t="n">
         <v>11.1</v>
       </c>
-      <c r="F132" t="inlineStr"/>
       <c r="G132" t="inlineStr"/>
       <c r="H132" t="n">
         <v>0.71152</v>
@@ -3792,10 +3792,10 @@
       <c r="D133" t="n">
         <v>-8.1</v>
       </c>
-      <c r="E133" t="n">
+      <c r="E133" t="inlineStr"/>
+      <c r="F133" t="n">
         <v>12.3</v>
       </c>
-      <c r="F133" t="inlineStr"/>
       <c r="G133" t="inlineStr"/>
       <c r="H133" t="inlineStr"/>
       <c r="I133" t="inlineStr">
@@ -3840,10 +3840,10 @@
       <c r="D135" t="n">
         <v>-8.9</v>
       </c>
-      <c r="E135" t="n">
+      <c r="E135" t="inlineStr"/>
+      <c r="F135" t="n">
         <v>12.6</v>
       </c>
-      <c r="F135" t="inlineStr"/>
       <c r="G135" t="inlineStr"/>
       <c r="H135" t="n">
         <v>0.7385699999999999</v>
@@ -3938,10 +3938,10 @@
       <c r="D139" t="n">
         <v>-7.3</v>
       </c>
-      <c r="E139" t="n">
+      <c r="E139" t="inlineStr"/>
+      <c r="F139" t="n">
         <v>11.1</v>
       </c>
-      <c r="F139" t="inlineStr"/>
       <c r="G139" t="inlineStr"/>
       <c r="H139" t="n">
         <v>0.71128</v>
@@ -4178,13 +4178,13 @@
       <c r="D149" t="n">
         <v>-8.800000000000001</v>
       </c>
-      <c r="E149" t="n">
+      <c r="E149" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+      <c r="F149" t="n">
         <v>8.1</v>
-      </c>
-      <c r="F149" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
       </c>
       <c r="G149" t="inlineStr"/>
       <c r="H149" t="n">
@@ -4258,10 +4258,10 @@
         <v>-5</v>
       </c>
       <c r="E152" t="n">
+        <v>17.38</v>
+      </c>
+      <c r="F152" t="n">
         <v>7.8</v>
-      </c>
-      <c r="F152" t="n">
-        <v>17.38</v>
       </c>
       <c r="G152" t="inlineStr"/>
       <c r="H152" t="n">
@@ -4332,10 +4332,10 @@
       <c r="D155" t="n">
         <v>-7.6</v>
       </c>
-      <c r="E155" t="n">
+      <c r="E155" t="inlineStr"/>
+      <c r="F155" t="n">
         <v>10.3</v>
       </c>
-      <c r="F155" t="inlineStr"/>
       <c r="G155" t="inlineStr"/>
       <c r="H155" t="inlineStr"/>
       <c r="I155" t="inlineStr">
@@ -4357,10 +4357,10 @@
       <c r="D156" t="n">
         <v>-9.800000000000001</v>
       </c>
-      <c r="E156" t="n">
+      <c r="E156" t="inlineStr"/>
+      <c r="F156" t="n">
         <v>8.800000000000001</v>
       </c>
-      <c r="F156" t="inlineStr"/>
       <c r="G156" t="inlineStr"/>
       <c r="H156" t="inlineStr"/>
       <c r="I156" t="inlineStr">
@@ -4382,10 +4382,10 @@
       <c r="D157" t="n">
         <v>-6</v>
       </c>
-      <c r="E157" t="n">
+      <c r="E157" t="inlineStr"/>
+      <c r="F157" t="n">
         <v>13.8</v>
       </c>
-      <c r="F157" t="inlineStr"/>
       <c r="G157" t="inlineStr"/>
       <c r="H157" t="inlineStr"/>
       <c r="I157" t="inlineStr">
@@ -4407,10 +4407,10 @@
       <c r="D158" t="n">
         <v>-7.4</v>
       </c>
-      <c r="E158" t="n">
+      <c r="E158" t="inlineStr"/>
+      <c r="F158" t="n">
         <v>7</v>
       </c>
-      <c r="F158" t="inlineStr"/>
       <c r="G158" t="inlineStr"/>
       <c r="H158" t="inlineStr"/>
       <c r="I158" t="inlineStr">
@@ -4526,10 +4526,10 @@
       <c r="D163" t="n">
         <v>-8.6</v>
       </c>
-      <c r="E163" t="n">
+      <c r="E163" t="inlineStr"/>
+      <c r="F163" t="n">
         <v>11.7</v>
       </c>
-      <c r="F163" t="inlineStr"/>
       <c r="G163" t="inlineStr"/>
       <c r="H163" t="inlineStr"/>
       <c r="I163" t="inlineStr">
@@ -4552,10 +4552,10 @@
         <v>-6.3</v>
       </c>
       <c r="E164" t="n">
+        <v>17.22</v>
+      </c>
+      <c r="F164" t="n">
         <v>12.7</v>
-      </c>
-      <c r="F164" t="n">
-        <v>17.22</v>
       </c>
       <c r="G164" t="inlineStr"/>
       <c r="H164" t="n">
@@ -4603,10 +4603,10 @@
       <c r="D166" t="n">
         <v>-6.3</v>
       </c>
-      <c r="E166" t="n">
+      <c r="E166" t="inlineStr"/>
+      <c r="F166" t="n">
         <v>11.7</v>
       </c>
-      <c r="F166" t="inlineStr"/>
       <c r="G166" t="inlineStr"/>
       <c r="H166" t="inlineStr"/>
       <c r="I166" t="inlineStr">
@@ -4652,10 +4652,10 @@
         <v>-10</v>
       </c>
       <c r="E168" t="n">
+        <v>17</v>
+      </c>
+      <c r="F168" t="n">
         <v>13.2</v>
-      </c>
-      <c r="F168" t="n">
-        <v>17</v>
       </c>
       <c r="G168" t="inlineStr"/>
       <c r="H168" t="n">
@@ -4705,10 +4705,10 @@
       <c r="D170" t="n">
         <v>-7.1</v>
       </c>
-      <c r="E170" t="n">
+      <c r="E170" t="inlineStr"/>
+      <c r="F170" t="n">
         <v>4.2</v>
       </c>
-      <c r="F170" t="inlineStr"/>
       <c r="G170" t="inlineStr"/>
       <c r="H170" t="inlineStr"/>
       <c r="I170" t="inlineStr">
@@ -4731,10 +4731,10 @@
         <v>-5.9</v>
       </c>
       <c r="E171" t="n">
+        <v>17.44</v>
+      </c>
+      <c r="F171" t="n">
         <v>14</v>
-      </c>
-      <c r="F171" t="n">
-        <v>17.44</v>
       </c>
       <c r="G171" t="inlineStr"/>
       <c r="H171" t="n">
@@ -4782,10 +4782,10 @@
       <c r="D173" t="n">
         <v>-6.8</v>
       </c>
-      <c r="E173" t="inlineStr"/>
-      <c r="F173" t="n">
+      <c r="E173" t="n">
         <v>18.06</v>
       </c>
+      <c r="F173" t="inlineStr"/>
       <c r="G173" t="inlineStr"/>
       <c r="H173" t="n">
         <v>0.70951</v>
@@ -4809,10 +4809,10 @@
       <c r="D174" t="n">
         <v>-5.7</v>
       </c>
-      <c r="E174" t="inlineStr"/>
-      <c r="F174" t="n">
+      <c r="E174" t="n">
         <v>16.89</v>
       </c>
+      <c r="F174" t="inlineStr"/>
       <c r="G174" t="inlineStr"/>
       <c r="H174" t="n">
         <v>0.71096</v>
@@ -4836,10 +4836,10 @@
       <c r="D175" t="n">
         <v>-8.1</v>
       </c>
-      <c r="E175" t="inlineStr"/>
-      <c r="F175" t="n">
+      <c r="E175" t="n">
         <v>17.18</v>
       </c>
+      <c r="F175" t="inlineStr"/>
       <c r="G175" t="inlineStr"/>
       <c r="H175" t="n">
         <v>0.70948</v>
@@ -4863,10 +4863,10 @@
       <c r="D176" t="n">
         <v>-8.6</v>
       </c>
-      <c r="E176" t="n">
+      <c r="E176" t="inlineStr"/>
+      <c r="F176" t="n">
         <v>12.1</v>
       </c>
-      <c r="F176" t="inlineStr"/>
       <c r="G176" t="inlineStr"/>
       <c r="H176" t="inlineStr"/>
       <c r="I176" t="inlineStr">
@@ -4911,10 +4911,10 @@
       <c r="D178" t="n">
         <v>-7.6</v>
       </c>
-      <c r="E178" t="n">
+      <c r="E178" t="inlineStr"/>
+      <c r="F178" t="n">
         <v>12</v>
       </c>
-      <c r="F178" t="inlineStr"/>
       <c r="G178" t="inlineStr"/>
       <c r="H178" t="inlineStr"/>
       <c r="I178" t="inlineStr">
@@ -5005,10 +5005,10 @@
       <c r="D182" t="n">
         <v>-7.6</v>
       </c>
-      <c r="E182" t="n">
+      <c r="E182" t="inlineStr"/>
+      <c r="F182" t="n">
         <v>12.4</v>
       </c>
-      <c r="F182" t="inlineStr"/>
       <c r="G182" t="inlineStr"/>
       <c r="H182" t="inlineStr"/>
       <c r="I182" t="inlineStr">
@@ -5076,10 +5076,10 @@
       <c r="D185" t="n">
         <v>-6.4</v>
       </c>
-      <c r="E185" t="inlineStr"/>
-      <c r="F185" t="n">
+      <c r="E185" t="n">
         <v>17.39</v>
       </c>
+      <c r="F185" t="inlineStr"/>
       <c r="G185" t="inlineStr"/>
       <c r="H185" t="n">
         <v>0.71183</v>
@@ -5126,10 +5126,10 @@
       <c r="D187" t="n">
         <v>-6.2</v>
       </c>
-      <c r="E187" t="n">
+      <c r="E187" t="inlineStr"/>
+      <c r="F187" t="n">
         <v>11.3</v>
       </c>
-      <c r="F187" t="inlineStr"/>
       <c r="G187" t="inlineStr"/>
       <c r="H187" t="inlineStr"/>
       <c r="I187" t="inlineStr">
@@ -5220,10 +5220,10 @@
       <c r="D191" t="n">
         <v>-10.1</v>
       </c>
-      <c r="E191" t="n">
+      <c r="E191" t="inlineStr"/>
+      <c r="F191" t="n">
         <v>11.6</v>
       </c>
-      <c r="F191" t="inlineStr"/>
       <c r="G191" t="inlineStr"/>
       <c r="H191" t="inlineStr"/>
       <c r="I191" t="inlineStr">
@@ -5245,10 +5245,10 @@
       <c r="D192" t="n">
         <v>-7.5</v>
       </c>
-      <c r="E192" t="n">
+      <c r="E192" t="inlineStr"/>
+      <c r="F192" t="n">
         <v>12.1</v>
       </c>
-      <c r="F192" t="inlineStr"/>
       <c r="G192" t="inlineStr"/>
       <c r="H192" t="inlineStr"/>
       <c r="I192" t="inlineStr">
@@ -5270,10 +5270,10 @@
       <c r="D193" t="n">
         <v>-8.800000000000001</v>
       </c>
-      <c r="E193" t="n">
+      <c r="E193" t="inlineStr"/>
+      <c r="F193" t="n">
         <v>11.3</v>
       </c>
-      <c r="F193" t="inlineStr"/>
       <c r="G193" t="inlineStr"/>
       <c r="H193" t="inlineStr"/>
       <c r="I193" t="inlineStr">
@@ -5295,10 +5295,10 @@
       <c r="D194" t="n">
         <v>-6.2</v>
       </c>
-      <c r="E194" t="n">
+      <c r="E194" t="inlineStr"/>
+      <c r="F194" t="n">
         <v>12.2</v>
       </c>
-      <c r="F194" t="inlineStr"/>
       <c r="G194" t="inlineStr"/>
       <c r="H194" t="inlineStr"/>
       <c r="I194" t="inlineStr">
@@ -5320,10 +5320,10 @@
       <c r="D195" t="n">
         <v>-6.1</v>
       </c>
-      <c r="E195" t="n">
+      <c r="E195" t="inlineStr"/>
+      <c r="F195" t="n">
         <v>12.2</v>
       </c>
-      <c r="F195" t="inlineStr"/>
       <c r="G195" t="inlineStr"/>
       <c r="H195" t="inlineStr"/>
       <c r="I195" t="inlineStr">
@@ -5345,10 +5345,10 @@
       <c r="D196" t="n">
         <v>-7.2</v>
       </c>
-      <c r="E196" t="n">
+      <c r="E196" t="inlineStr"/>
+      <c r="F196" t="n">
         <v>12.2</v>
       </c>
-      <c r="F196" t="inlineStr"/>
       <c r="G196" t="inlineStr"/>
       <c r="H196" t="inlineStr"/>
       <c r="I196" t="inlineStr">
@@ -5371,10 +5371,10 @@
         <v>-10.7</v>
       </c>
       <c r="E197" t="n">
+        <v>17.53</v>
+      </c>
+      <c r="F197" t="n">
         <v>11.9</v>
-      </c>
-      <c r="F197" t="n">
-        <v>17.53</v>
       </c>
       <c r="G197" t="inlineStr"/>
       <c r="H197" t="n">
@@ -5399,10 +5399,10 @@
       <c r="D198" t="n">
         <v>-7.6</v>
       </c>
-      <c r="E198" t="n">
+      <c r="E198" t="inlineStr"/>
+      <c r="F198" t="n">
         <v>12.3</v>
       </c>
-      <c r="F198" t="inlineStr"/>
       <c r="G198" t="inlineStr"/>
       <c r="H198" t="inlineStr"/>
       <c r="I198" t="inlineStr">
@@ -5424,10 +5424,10 @@
       <c r="D199" t="n">
         <v>-7.7</v>
       </c>
-      <c r="E199" t="n">
+      <c r="E199" t="inlineStr"/>
+      <c r="F199" t="n">
         <v>12.4</v>
       </c>
-      <c r="F199" t="inlineStr"/>
       <c r="G199" t="inlineStr"/>
       <c r="H199" t="inlineStr"/>
       <c r="I199" t="inlineStr">
@@ -5449,10 +5449,10 @@
       <c r="D200" t="n">
         <v>-7.6</v>
       </c>
-      <c r="E200" t="n">
+      <c r="E200" t="inlineStr"/>
+      <c r="F200" t="n">
         <v>9.699999999999999</v>
       </c>
-      <c r="F200" t="inlineStr"/>
       <c r="G200" t="inlineStr"/>
       <c r="H200" t="inlineStr"/>
       <c r="I200" t="inlineStr">

</xml_diff>